<commit_message>
alpha: full for UTM only
mathon - nov 11, 2025
---
added feature to extract actual processed dates for UTM only - UTE and UTA not implemented but ready for
</commit_message>
<xml_diff>
--- a/Avanzamento_schede_automated.xlsx
+++ b/Avanzamento_schede_automated.xlsx
@@ -805,6 +805,9 @@
       <c r="Y2" s="9" t="n">
         <v>45926</v>
       </c>
+      <c r="Z2" s="9" t="n">
+        <v>45926</v>
+      </c>
     </row>
     <row r="3" ht="16.5" customHeight="1">
       <c r="A3" s="5" t="inlineStr">
@@ -849,6 +852,9 @@
       <c r="Y3" s="9" t="n">
         <v>45926</v>
       </c>
+      <c r="Z3" s="9" t="n">
+        <v>45926</v>
+      </c>
     </row>
     <row r="4" ht="16.5" customHeight="1">
       <c r="A4" s="5" t="inlineStr">
@@ -918,6 +924,9 @@
       <c r="Y4" s="9" t="n">
         <v>45912</v>
       </c>
+      <c r="Z4" s="9" t="n">
+        <v>45926</v>
+      </c>
     </row>
     <row r="5" ht="16.5" customHeight="1">
       <c r="A5" s="5" t="inlineStr">
@@ -999,6 +1008,9 @@
       <c r="Y5" s="9" t="n">
         <v>45800</v>
       </c>
+      <c r="Z5" s="9" t="n">
+        <v>45926</v>
+      </c>
     </row>
     <row r="6" ht="32.25" customHeight="1">
       <c r="A6" s="5" t="inlineStr">
@@ -1042,6 +1054,9 @@
         <v>45924</v>
       </c>
       <c r="Y6" s="9" t="n">
+        <v>45924</v>
+      </c>
+      <c r="Z6" s="9" t="n">
         <v>45924</v>
       </c>
     </row>
@@ -1107,6 +1122,9 @@
       <c r="Y7" s="9" t="n">
         <v>45926</v>
       </c>
+      <c r="Z7" s="9" t="n">
+        <v>45923</v>
+      </c>
     </row>
     <row r="8" ht="16.5" customHeight="1">
       <c r="A8" s="5" t="inlineStr">
@@ -1164,6 +1182,9 @@
       <c r="Y8" s="9" t="n">
         <v>45924</v>
       </c>
+      <c r="Z8" s="9" t="n">
+        <v>45922</v>
+      </c>
     </row>
     <row r="9" ht="16.5" customHeight="1">
       <c r="A9" s="5" t="inlineStr">
@@ -1215,6 +1236,9 @@
       <c r="Y9" s="9" t="n">
         <v>45922</v>
       </c>
+      <c r="Z9" s="9" t="n">
+        <v>45922</v>
+      </c>
     </row>
     <row r="10" ht="16.5" customHeight="1">
       <c r="A10" s="5" t="inlineStr">
@@ -1258,6 +1282,9 @@
         <v>45922</v>
       </c>
       <c r="Y10" s="9" t="n">
+        <v>45922</v>
+      </c>
+      <c r="Z10" s="9" t="n">
         <v>45922</v>
       </c>
     </row>
@@ -1338,6 +1365,9 @@
       <c r="Y11" s="9" t="n">
         <v>45777</v>
       </c>
+      <c r="Z11" s="9" t="n">
+        <v>45922</v>
+      </c>
     </row>
     <row r="12" ht="16.5" customHeight="1">
       <c r="A12" s="5" t="inlineStr">
@@ -1404,6 +1434,9 @@
       </c>
       <c r="Y12" s="9" t="n">
         <v>45917</v>
+      </c>
+      <c r="Z12" s="9" t="n">
+        <v>45919</v>
       </c>
     </row>
     <row r="13" ht="16.5" customHeight="1">
@@ -1486,6 +1519,9 @@
       <c r="Y13" s="9" t="n">
         <v>45845</v>
       </c>
+      <c r="Z13" s="9" t="n">
+        <v>45919</v>
+      </c>
     </row>
     <row r="14" ht="16.5" customHeight="1">
       <c r="A14" s="5" t="inlineStr">
@@ -1548,6 +1584,9 @@
       <c r="Y14" s="9" t="n">
         <v>45901</v>
       </c>
+      <c r="Z14" s="9" t="n">
+        <v>45918</v>
+      </c>
     </row>
     <row r="15" ht="16.5" customHeight="1">
       <c r="A15" s="5" t="inlineStr">
@@ -1609,6 +1648,9 @@
       </c>
       <c r="Y15" s="9" t="n">
         <v>45916</v>
+      </c>
+      <c r="Z15" s="9" t="n">
+        <v>45917</v>
       </c>
     </row>
     <row r="16" ht="16.5" customHeight="1">
@@ -1679,6 +1721,9 @@
       <c r="Y16" s="9" t="n">
         <v>45915</v>
       </c>
+      <c r="Z16" s="9" t="n">
+        <v>45916</v>
+      </c>
     </row>
     <row r="17" ht="16.5" customHeight="1">
       <c r="A17" s="5" t="inlineStr">
@@ -1736,6 +1781,9 @@
       <c r="Y17" s="9" t="n">
         <v>45916</v>
       </c>
+      <c r="Z17" s="9" t="n">
+        <v>45916</v>
+      </c>
     </row>
     <row r="18" ht="16.5" customHeight="1">
       <c r="A18" s="5" t="inlineStr">
@@ -1796,6 +1844,9 @@
       <c r="Y18" s="9" t="n">
         <v>45919</v>
       </c>
+      <c r="Z18" s="9" t="n">
+        <v>45915</v>
+      </c>
     </row>
     <row r="19" ht="16.5" customHeight="1">
       <c r="A19" s="5" t="inlineStr">
@@ -1859,6 +1910,9 @@
       <c r="Y19" s="9" t="n">
         <v>45915</v>
       </c>
+      <c r="Z19" s="9" t="n">
+        <v>45933</v>
+      </c>
     </row>
     <row r="20" ht="16.5" customHeight="1">
       <c r="A20" s="5" t="inlineStr">
@@ -1920,6 +1974,9 @@
       <c r="Y20" s="9" t="n">
         <v>45926</v>
       </c>
+      <c r="Z20" s="9" t="n">
+        <v>45915</v>
+      </c>
     </row>
     <row r="21" ht="16.5" customHeight="1">
       <c r="A21" s="5" t="inlineStr">
@@ -1958,6 +2015,9 @@
       </c>
       <c r="Y21" s="9" t="n">
         <v>45916</v>
+      </c>
+      <c r="Z21" s="9" t="n">
+        <v>45915</v>
       </c>
     </row>
     <row r="22" ht="16.5" customHeight="1">
@@ -2016,6 +2076,9 @@
       <c r="Y22" s="9" t="n">
         <v>45916</v>
       </c>
+      <c r="Z22" s="9" t="n">
+        <v>45915</v>
+      </c>
     </row>
     <row r="23" ht="16.5" customHeight="1">
       <c r="A23" s="5" t="inlineStr">
@@ -2064,6 +2127,9 @@
       <c r="Y23" s="9" t="n">
         <v>45915</v>
       </c>
+      <c r="Z23" s="9" t="n">
+        <v>45915</v>
+      </c>
     </row>
     <row r="24" ht="16.5" customHeight="1">
       <c r="A24" s="5" t="inlineStr">
@@ -2148,6 +2214,9 @@
       </c>
       <c r="Y24" s="9" t="n">
         <v>45908</v>
+      </c>
+      <c r="Z24" s="9" t="n">
+        <v>45912</v>
       </c>
     </row>
     <row r="25" ht="16.5" customHeight="1">
@@ -2199,6 +2268,9 @@
       <c r="Y25" s="9" t="n">
         <v>45919</v>
       </c>
+      <c r="Z25" s="9" t="n">
+        <v>45911</v>
+      </c>
     </row>
     <row r="26" ht="16.5" customHeight="1">
       <c r="A26" s="5" t="inlineStr">
@@ -2256,6 +2328,9 @@
       <c r="Y26" s="9" t="n">
         <v>45912</v>
       </c>
+      <c r="Z26" s="9" t="n">
+        <v>45911</v>
+      </c>
     </row>
     <row r="27" ht="16.5" customHeight="1">
       <c r="A27" s="5" t="inlineStr">
@@ -2316,6 +2391,9 @@
         <v>45909</v>
       </c>
       <c r="Y27" s="9" t="n">
+        <v>45909</v>
+      </c>
+      <c r="Z27" s="9" t="n">
         <v>45909</v>
       </c>
     </row>
@@ -2384,6 +2462,9 @@
       <c r="Y28" s="9" t="n">
         <v>45784</v>
       </c>
+      <c r="Z28" s="9" t="n">
+        <v>45909</v>
+      </c>
     </row>
     <row r="29" ht="16.5" customHeight="1">
       <c r="A29" s="5" t="inlineStr">
@@ -2440,6 +2521,9 @@
       </c>
       <c r="Y29" s="9" t="n">
         <v>45895</v>
+      </c>
+      <c r="Z29" s="9" t="n">
+        <v>45909</v>
       </c>
     </row>
     <row r="30" ht="16.5" customHeight="1">
@@ -2512,6 +2596,9 @@
       <c r="Y30" s="9" t="n">
         <v>45915</v>
       </c>
+      <c r="Z30" s="9" t="n">
+        <v>45909</v>
+      </c>
     </row>
     <row r="31" ht="16.5" customHeight="1">
       <c r="A31" s="5" t="inlineStr">
@@ -2577,6 +2664,9 @@
         <v>45909</v>
       </c>
       <c r="Y31" s="9" t="n">
+        <v>45909</v>
+      </c>
+      <c r="Z31" s="9" t="n">
         <v>45909</v>
       </c>
     </row>
@@ -2631,6 +2721,9 @@
       <c r="Y32" s="9" t="n">
         <v>45838</v>
       </c>
+      <c r="Z32" s="9" t="n">
+        <v>45909</v>
+      </c>
     </row>
     <row r="33" ht="16.5" customHeight="1">
       <c r="A33" s="5" t="inlineStr">
@@ -2696,6 +2789,9 @@
       <c r="Y33" s="9" t="n">
         <v>45908</v>
       </c>
+      <c r="Z33" s="9" t="n">
+        <v>45908</v>
+      </c>
     </row>
     <row r="34" ht="16.5" customHeight="1">
       <c r="A34" s="5" t="inlineStr">
@@ -2756,6 +2852,9 @@
       <c r="Y34" s="9" t="n">
         <v>45908</v>
       </c>
+      <c r="Z34" s="9" t="n">
+        <v>45908</v>
+      </c>
     </row>
     <row r="35" ht="16.5" customHeight="1">
       <c r="A35" s="5" t="inlineStr">
@@ -2815,6 +2914,9 @@
       <c r="Y35" s="9" t="n">
         <v>45908</v>
       </c>
+      <c r="Z35" s="9" t="n">
+        <v>45908</v>
+      </c>
     </row>
     <row r="36" ht="16.5" customHeight="1">
       <c r="A36" s="5" t="inlineStr">
@@ -2885,6 +2987,9 @@
       </c>
       <c r="Y36" s="9" t="n">
         <v>45912</v>
+      </c>
+      <c r="Z36" s="9" t="n">
+        <v>45937</v>
       </c>
     </row>
     <row r="37" ht="16.5" customHeight="1">
@@ -2931,6 +3036,9 @@
       <c r="Y37" s="9" t="n">
         <v>45856</v>
       </c>
+      <c r="Z37" s="9" t="n">
+        <v>45898</v>
+      </c>
     </row>
     <row r="38" ht="16.5" customHeight="1">
       <c r="A38" s="5" t="inlineStr">
@@ -3015,6 +3123,9 @@
       </c>
       <c r="Y38" s="9" t="n">
         <v>45909</v>
+      </c>
+      <c r="Z38" s="9" t="n">
+        <v>45897</v>
       </c>
     </row>
     <row r="39" ht="16.5" customHeight="1">
@@ -3088,6 +3199,9 @@
       <c r="Y39" s="9" t="n">
         <v>45897</v>
       </c>
+      <c r="Z39" s="9" t="n">
+        <v>45897</v>
+      </c>
     </row>
     <row r="40" ht="16.5" customHeight="1">
       <c r="A40" s="5" t="inlineStr">
@@ -3154,6 +3268,9 @@
       <c r="Y40" s="9" t="n">
         <v>45909</v>
       </c>
+      <c r="Z40" s="9" t="n">
+        <v>45897</v>
+      </c>
     </row>
     <row r="41" ht="16.5" customHeight="1">
       <c r="A41" s="5" t="inlineStr">
@@ -3208,6 +3325,9 @@
       <c r="Y41" s="9" t="n">
         <v>45902</v>
       </c>
+      <c r="Z41" s="9" t="n">
+        <v>45897</v>
+      </c>
     </row>
     <row r="42" ht="16.5" customHeight="1">
       <c r="A42" s="5" t="inlineStr">
@@ -3292,6 +3412,9 @@
       </c>
       <c r="Y42" s="9" t="n">
         <v>45908</v>
+      </c>
+      <c r="Z42" s="9" t="n">
+        <v>45897</v>
       </c>
     </row>
     <row r="43" ht="16.5" customHeight="1">
@@ -3374,6 +3497,9 @@
       <c r="Y43" s="9" t="n">
         <v>45845</v>
       </c>
+      <c r="Z43" s="9" t="n">
+        <v>45863</v>
+      </c>
     </row>
     <row r="44" ht="16.5" customHeight="1">
       <c r="A44" s="5" t="inlineStr">
@@ -3443,6 +3569,9 @@
       <c r="Y44" s="9" t="n">
         <v>45902</v>
       </c>
+      <c r="Z44" s="9" t="n">
+        <v>45896</v>
+      </c>
     </row>
     <row r="45" ht="16.5" customHeight="1">
       <c r="A45" s="5" t="inlineStr">
@@ -3492,6 +3621,9 @@
       <c r="Y45" s="9" t="n">
         <v>45883</v>
       </c>
+      <c r="Z45" s="9" t="n">
+        <v>45887</v>
+      </c>
     </row>
     <row r="46" ht="16.5" customHeight="1">
       <c r="A46" s="5" t="inlineStr">
@@ -3562,6 +3694,9 @@
       <c r="Y46" s="9" t="n">
         <v>45908</v>
       </c>
+      <c r="Z46" s="9" t="n">
+        <v>45887</v>
+      </c>
     </row>
     <row r="47" ht="16.5" customHeight="1">
       <c r="A47" s="5" t="inlineStr">
@@ -3635,6 +3770,9 @@
       <c r="Y47" s="9" t="n">
         <v>45887</v>
       </c>
+      <c r="Z47" s="9" t="n">
+        <v>45887</v>
+      </c>
     </row>
     <row r="48" ht="16.5" customHeight="1">
       <c r="A48" s="5" t="inlineStr">
@@ -3702,6 +3840,9 @@
       <c r="Y48" s="9" t="n">
         <v>45895</v>
       </c>
+      <c r="Z48" s="9" t="n">
+        <v>45887</v>
+      </c>
     </row>
     <row r="49" ht="16.5" customHeight="1">
       <c r="A49" s="5" t="inlineStr">
@@ -3740,6 +3881,9 @@
         <is>
           <t>KOM</t>
         </is>
+      </c>
+      <c r="Z49" s="9" t="n">
+        <v>45887</v>
       </c>
     </row>
     <row r="50" ht="16.5" customHeight="1">
@@ -3813,6 +3957,9 @@
       <c r="Y50" s="9" t="n">
         <v>45748</v>
       </c>
+      <c r="Z50" s="9" t="n">
+        <v>45887</v>
+      </c>
     </row>
     <row r="51" ht="16.5" customHeight="1">
       <c r="A51" s="5" t="inlineStr">
@@ -3886,6 +4033,9 @@
         <v>45876</v>
       </c>
       <c r="Y51" s="9" t="n">
+        <v>45876</v>
+      </c>
+      <c r="Z51" s="9" t="n">
         <v>45876</v>
       </c>
     </row>
@@ -3946,6 +4096,9 @@
       <c r="Y52" s="9" t="n">
         <v>45874</v>
       </c>
+      <c r="Z52" s="9" t="n">
+        <v>45874</v>
+      </c>
     </row>
     <row r="53" ht="16.5" customHeight="1">
       <c r="A53" s="5" t="inlineStr">
@@ -4027,6 +4180,9 @@
       <c r="Y53" s="9" t="n">
         <v>45840</v>
       </c>
+      <c r="Z53" s="9" t="n">
+        <v>45873</v>
+      </c>
     </row>
     <row r="54" ht="16.5" customHeight="1">
       <c r="A54" s="5" t="inlineStr">
@@ -4108,6 +4264,9 @@
       <c r="Y54" s="9" t="n">
         <v>45870</v>
       </c>
+      <c r="Z54" s="9" t="n">
+        <v>45870</v>
+      </c>
     </row>
     <row r="55" ht="32.25" customHeight="1">
       <c r="A55" s="5" t="inlineStr">
@@ -4181,6 +4340,9 @@
       </c>
       <c r="Y55" s="9" t="n">
         <v>45873</v>
+      </c>
+      <c r="Z55" s="9" t="n">
+        <v>45870</v>
       </c>
     </row>
     <row r="56" ht="16.5" customHeight="1">
@@ -4263,6 +4425,9 @@
       <c r="Y56" s="9" t="n">
         <v>45797</v>
       </c>
+      <c r="Z56" s="9" t="n">
+        <v>45869</v>
+      </c>
     </row>
     <row r="57" ht="16.5" customHeight="1">
       <c r="A57" s="5" t="inlineStr">
@@ -4328,6 +4493,9 @@
       <c r="Y57" s="9" t="n">
         <v>45869</v>
       </c>
+      <c r="Z57" s="9" t="n">
+        <v>45869</v>
+      </c>
     </row>
     <row r="58" ht="16.5" customHeight="1">
       <c r="A58" s="5" t="inlineStr">
@@ -4390,6 +4558,9 @@
       <c r="Y58" s="9" t="n">
         <v>45869</v>
       </c>
+      <c r="Z58" s="9" t="n">
+        <v>45869</v>
+      </c>
     </row>
     <row r="59" ht="16.5" customHeight="1">
       <c r="A59" s="5" t="inlineStr">
@@ -4444,6 +4615,9 @@
         <v>45869</v>
       </c>
       <c r="Y59" s="9" t="n">
+        <v>45869</v>
+      </c>
+      <c r="Z59" s="9" t="n">
         <v>45869</v>
       </c>
     </row>
@@ -4527,6 +4701,9 @@
       <c r="Y60" s="9" t="n">
         <v>45803</v>
       </c>
+      <c r="Z60" s="9" t="n">
+        <v>45867</v>
+      </c>
     </row>
     <row r="61" ht="16.5" customHeight="1">
       <c r="A61" s="5" t="inlineStr">
@@ -4602,6 +4779,9 @@
       <c r="Y61" s="9" t="n">
         <v>45876</v>
       </c>
+      <c r="Z61" s="9" t="n">
+        <v>45866</v>
+      </c>
     </row>
     <row r="62" ht="16.5" customHeight="1">
       <c r="A62" s="5" t="inlineStr">
@@ -4672,6 +4852,9 @@
       <c r="Y62" s="9" t="n">
         <v>45866</v>
       </c>
+      <c r="Z62" s="9" t="n">
+        <v>45866</v>
+      </c>
     </row>
     <row r="63" ht="16.5" customHeight="1">
       <c r="A63" s="5" t="inlineStr">
@@ -4737,6 +4920,9 @@
       <c r="Y63" s="9" t="n">
         <v>45866</v>
       </c>
+      <c r="Z63" s="9" t="n">
+        <v>45866</v>
+      </c>
     </row>
     <row r="64" ht="16.5" customHeight="1">
       <c r="A64" s="5" t="inlineStr">
@@ -4802,6 +4988,9 @@
       <c r="Y64" s="9" t="n">
         <v>45866</v>
       </c>
+      <c r="Z64" s="9" t="n">
+        <v>45866</v>
+      </c>
     </row>
     <row r="65" ht="16.5" customHeight="1">
       <c r="A65" s="5" t="inlineStr">
@@ -4883,6 +5072,9 @@
       <c r="Y65" s="9" t="n">
         <v>45863</v>
       </c>
+      <c r="Z65" s="9" t="n">
+        <v>45863</v>
+      </c>
     </row>
     <row r="66" ht="16.5" customHeight="1">
       <c r="A66" s="5" t="inlineStr">
@@ -4964,6 +5156,9 @@
       <c r="Y66" s="9" t="n">
         <v>45856</v>
       </c>
+      <c r="Z66" s="9" t="n">
+        <v>45862</v>
+      </c>
     </row>
     <row r="67" ht="16.5" customHeight="1">
       <c r="A67" s="5" t="inlineStr">
@@ -4992,6 +5187,9 @@
       <c r="F67" s="13" t="n"/>
       <c r="G67" s="6" t="n"/>
       <c r="H67" s="5" t="n"/>
+      <c r="Z67" s="9" t="n">
+        <v>45860</v>
+      </c>
     </row>
     <row r="68" ht="16.5" customHeight="1">
       <c r="A68" s="5" t="inlineStr">
@@ -5065,6 +5263,9 @@
       <c r="Y68" s="9" t="n">
         <v>45838</v>
       </c>
+      <c r="Z68" s="9" t="n">
+        <v>45860</v>
+      </c>
     </row>
     <row r="69" ht="16.5" customHeight="1">
       <c r="A69" s="5" t="inlineStr">
@@ -5110,6 +5311,9 @@
       <c r="Y69" s="9" t="n">
         <v>45968</v>
       </c>
+      <c r="Z69" s="9" t="n">
+        <v>45860</v>
+      </c>
     </row>
     <row r="70" ht="16.5" customHeight="1">
       <c r="A70" s="5" t="inlineStr">
@@ -5188,6 +5392,9 @@
       <c r="Y70" s="9" t="n">
         <v>45861</v>
       </c>
+      <c r="Z70" s="9" t="n">
+        <v>45859</v>
+      </c>
     </row>
     <row r="71" ht="16.5" customHeight="1">
       <c r="A71" s="5" t="inlineStr">
@@ -5269,6 +5476,9 @@
       <c r="Y71" s="9" t="n">
         <v>45870</v>
       </c>
+      <c r="Z71" s="9" t="n">
+        <v>45859</v>
+      </c>
     </row>
     <row r="72" ht="16.5" customHeight="1">
       <c r="A72" s="5" t="inlineStr">
@@ -5309,6 +5519,9 @@
       <c r="Y72" s="9" t="n">
         <v>45856</v>
       </c>
+      <c r="Z72" s="9" t="n">
+        <v>45855</v>
+      </c>
     </row>
     <row r="73" ht="16.5" customHeight="1">
       <c r="A73" s="5" t="inlineStr">
@@ -5354,6 +5567,9 @@
       <c r="Y73" s="9" t="n">
         <v>45856</v>
       </c>
+      <c r="Z73" s="9" t="n">
+        <v>45854</v>
+      </c>
     </row>
     <row r="74" ht="16.5" customHeight="1">
       <c r="A74" s="5" t="inlineStr">
@@ -5386,6 +5602,9 @@
         <is>
           <t>KOM</t>
         </is>
+      </c>
+      <c r="Z74" s="9" t="n">
+        <v>45854</v>
       </c>
     </row>
     <row r="75" ht="16.5" customHeight="1">
@@ -5462,6 +5681,9 @@
       <c r="Y75" s="9" t="n">
         <v>45855</v>
       </c>
+      <c r="Z75" s="9" t="n">
+        <v>45854</v>
+      </c>
     </row>
     <row r="76" ht="16.5" customHeight="1">
       <c r="A76" s="5" t="inlineStr">
@@ -5543,6 +5765,9 @@
       <c r="Y76" s="9" t="n">
         <v>45845</v>
       </c>
+      <c r="Z76" s="9" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="77" ht="16.5" customHeight="1">
       <c r="A77" s="5" t="inlineStr">
@@ -5624,6 +5849,9 @@
       <c r="Y77" s="9" t="n">
         <v>45848</v>
       </c>
+      <c r="Z77" s="9" t="n">
+        <v>45853</v>
+      </c>
     </row>
     <row r="78" ht="16.5" customHeight="1">
       <c r="A78" s="5" t="inlineStr">
@@ -5699,6 +5927,9 @@
       </c>
       <c r="Y78" s="9" t="n">
         <v>45860</v>
+      </c>
+      <c r="Z78" s="9" t="n">
+        <v>45852</v>
       </c>
     </row>
     <row r="79" ht="16.5" customHeight="1">
@@ -5781,6 +6012,9 @@
       <c r="Y79" s="9" t="n">
         <v>45852</v>
       </c>
+      <c r="Z79" s="9" t="n">
+        <v>45852</v>
+      </c>
     </row>
     <row r="80" ht="16.5" customHeight="1">
       <c r="A80" s="5" t="inlineStr">
@@ -5820,6 +6054,9 @@
       </c>
       <c r="Y80" s="9" t="n">
         <v>45853</v>
+      </c>
+      <c r="Z80" s="9" t="n">
+        <v>45852</v>
       </c>
     </row>
     <row r="81" ht="16.5" customHeight="1">
@@ -5882,6 +6119,9 @@
       <c r="Y81" s="9" t="n">
         <v>45852</v>
       </c>
+      <c r="Z81" s="9" t="n">
+        <v>45852</v>
+      </c>
     </row>
     <row r="82" ht="16.5" customHeight="1">
       <c r="A82" s="5" t="inlineStr">
@@ -5943,6 +6183,9 @@
       <c r="Y82" s="9" t="n">
         <v>45846</v>
       </c>
+      <c r="Z82" s="9" t="n">
+        <v>45852</v>
+      </c>
     </row>
     <row r="83" ht="16.5" customHeight="1">
       <c r="A83" s="5" t="inlineStr">
@@ -6004,6 +6247,9 @@
       <c r="Y83" s="9" t="n">
         <v>45848</v>
       </c>
+      <c r="Z83" s="9" t="n">
+        <v>45852</v>
+      </c>
     </row>
     <row r="84" ht="16.5" customHeight="1">
       <c r="A84" s="5" t="inlineStr">
@@ -6050,6 +6296,9 @@
       <c r="Y84" s="9" t="n">
         <v>45849</v>
       </c>
+      <c r="Z84" s="9" t="n">
+        <v>45849</v>
+      </c>
     </row>
     <row r="85" ht="16.5" customHeight="1">
       <c r="A85" s="5" t="inlineStr">
@@ -6129,6 +6378,9 @@
       <c r="Y85" s="9" t="n">
         <v>45847</v>
       </c>
+      <c r="Z85" s="9" t="n">
+        <v>45848</v>
+      </c>
     </row>
     <row r="86" ht="16.5" customHeight="1">
       <c r="A86" s="5" t="inlineStr">
@@ -6201,6 +6453,9 @@
       <c r="Y86" s="9" t="n">
         <v>45847</v>
       </c>
+      <c r="Z86" s="9" t="n">
+        <v>45845</v>
+      </c>
     </row>
     <row r="87" ht="16.5" customHeight="1">
       <c r="A87" s="5" t="inlineStr">
@@ -6272,6 +6527,9 @@
       <c r="Y87" s="9" t="n">
         <v>45842</v>
       </c>
+      <c r="Z87" s="9" t="n">
+        <v>45841</v>
+      </c>
     </row>
     <row r="88" ht="16.5" customHeight="1">
       <c r="A88" s="5" t="inlineStr">
@@ -6349,6 +6607,9 @@
       <c r="Y88" s="9" t="n">
         <v>45840</v>
       </c>
+      <c r="Z88" s="9" t="n">
+        <v>45840</v>
+      </c>
     </row>
     <row r="89" ht="16.5" customHeight="1">
       <c r="A89" s="5" t="inlineStr">
@@ -6397,6 +6658,9 @@
       <c r="Y89" s="9" t="n">
         <v>45839</v>
       </c>
+      <c r="Z89" s="9" t="n">
+        <v>45839</v>
+      </c>
     </row>
     <row r="90" ht="16.5" customHeight="1">
       <c r="A90" s="5" t="inlineStr">
@@ -6427,6 +6691,9 @@
       <c r="Y90" s="9" t="n">
         <v>45765</v>
       </c>
+      <c r="Z90" s="9" t="n">
+        <v>45839</v>
+      </c>
     </row>
     <row r="91" ht="16.5" customHeight="1">
       <c r="A91" s="5" t="inlineStr">
@@ -6511,6 +6778,9 @@
       </c>
       <c r="Y91" s="9" t="n">
         <v>45842</v>
+      </c>
+      <c r="Z91" s="9" t="n">
+        <v>45839</v>
       </c>
     </row>
   </sheetData>

</xml_diff>